<commit_message>
Added screen shots for EB
</commit_message>
<xml_diff>
--- a/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/EB_SignalIndicator_JS.xlsx
+++ b/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/EB_SignalIndicator_JS.xlsx
@@ -479,24 +479,6 @@
 };</t>
   </si>
   <si>
-    <t>wait(3);
-validate1;
-SwitchApp(NATIVE_APP);
-ClickNativeIcon(VT200_0851_home_xpath);
-SwitchApp(WEBVIEW);
-link_Click(signal_test_link);
-validate2;
-SelectTestToRun(VT200_0851_string);
-ClickRunTest(runtest_top_xpath);
-validate3;
-ClickRunTest(runtest_bottom_xpath);
-wait(2);
-TakeScreenshot(VT200-0851);
-validate4;
-wait(2);
-TakeScreenshot(VT200-0851);</t>
-  </si>
-  <si>
     <t>validate1
 {
 validate_PageTitle=Compliance JS specs
@@ -585,6 +567,19 @@
 ChangeConfigxml(Configuration,WebServer,&lt;WebServer&gt;endl  &lt;Enabled VALUE="1"/&gt;endl  &lt;Port VALUE="8082"/&gt;endl  &lt;WebFolder VALUE="\\auto\\ComplianceTest_JS\"/&gt;endl  &lt;Public VALUE="1"/&gt;endl&lt;/WebServer&gt;endl);
 ChangeConfigxml(Configuration/Screen,FullScreen,&lt;FullScreen value="0"/&gt;);
 PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(3);
+validate1;
+link_Click(signal_test_link);
+validate2;
+SelectTestToRun(VT200_0851_string);
+ClickRunTest(runtest_top_xpath);
+validate3;
+ClickRunTest(runtest_bottom_xpath);
+wait(2);
+TakeScreenshot(VT200-0851);
+validate4;</t>
   </si>
 </sst>
 </file>
@@ -1001,9 +996,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -1062,13 +1055,13 @@
         <v>10</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F2" s="1">
         <v>1</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H2" s="5"/>
       <c r="I2" s="2" t="s">
@@ -1077,7 +1070,7 @@
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:11" ht="192" thickBot="1">
+    <row r="3" spans="1:11" ht="180.75" thickBot="1">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1095,7 +1088,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>41</v>
@@ -1122,7 +1115,7 @@
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>42</v>
@@ -1206,7 +1199,7 @@
         <v>28</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
@@ -1392,7 +1385,7 @@
         <v>1</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>45</v>
@@ -1419,7 +1412,7 @@
         <v>1</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>43</v>

</xml_diff>